<commit_message>
fixed a bug with the duplicate checker
</commit_message>
<xml_diff>
--- a/data/snapshots/3252783/xlsx/creators.xlsx
+++ b/data/snapshots/3252783/xlsx/creators.xlsx
@@ -405,7 +405,7 @@
         <v>stars1satwv984d3s0kmvnlh4wnf0enh5xwgaq3jzfdd</v>
       </c>
       <c r="B2">
-        <v>34755.319052</v>
+        <v>35159.619052</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -445,7 +445,7 @@
         <v>stars1sr7p3esz5xjsezzwrk6ec5hz2675jr692mzjul</v>
       </c>
       <c r="B4">
-        <v>1190.680996</v>
+        <v>1340.040996</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -545,7 +545,7 @@
         <v>stars1d6s8v9kp4jc9qj5u9c4mrl36tss4q7ydgezre7</v>
       </c>
       <c r="B9">
-        <v>1.02247</v>
+        <v>0.995319</v>
       </c>
       <c r="C9">
         <v>70000</v>
@@ -565,7 +565,7 @@
         <v>stars1uts2zr7lx2ln0v2rvzlx8ud2tfcya552my5h2e</v>
       </c>
       <c r="B10">
-        <v>43.70195</v>
+        <v>44.70195</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -605,7 +605,7 @@
         <v>stars1rlmqjkqtp4ctk4tw05vr08zvym7s5vyhvqpknw</v>
       </c>
       <c r="B12">
-        <v>44145.146773</v>
+        <v>44171.326773</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -645,10 +645,10 @@
         <v>stars1a67z7gyczt0npk24xpyy6ufx6l5gu546ah4l3u</v>
       </c>
       <c r="B14">
-        <v>6.151354</v>
+        <v>6.260751</v>
       </c>
       <c r="C14">
-        <v>13037.047524</v>
+        <v>13071.753763</v>
       </c>
       <c r="D14" t="str">
         <v>stars1jy9dagaycutdcjf99tp9uhl5ev9lykegp2tph6r9vu6xg3td6krs7agujy</v>
@@ -665,7 +665,7 @@
         <v>stars1zja6krwtcaa2ushn3z2m658k38qlg9qwg8casg</v>
       </c>
       <c r="B15">
-        <v>4318.208485</v>
+        <v>2199.204126</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -685,7 +685,7 @@
         <v>stars1easmle9uweupe525avpzjulumcyf52y6maqysh</v>
       </c>
       <c r="B16">
-        <v>150.281764</v>
+        <v>251.181764</v>
       </c>
       <c r="C16">
         <v>50</v>
@@ -705,10 +705,10 @@
         <v>stars1axw88ugkakle6g6ma7ev4f30lhzzyfaz3rus5u</v>
       </c>
       <c r="B17">
-        <v>92394.049727</v>
+        <v>75313.301416</v>
       </c>
       <c r="C17">
-        <v>273329.594594</v>
+        <v>298329.594594</v>
       </c>
       <c r="D17" t="str">
         <v>stars1ywpctek72gsccmr8gjgaamzs8vhh7ju3sjtvwk82daafavw5u0es293t0m</v>
@@ -725,7 +725,7 @@
         <v>stars1haql8s8dnn02nz5xjrwmamhskquz3aheqsjafq</v>
       </c>
       <c r="B18">
-        <v>383.008032</v>
+        <v>203.008032</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -765,7 +765,7 @@
         <v>stars19kh5z7ujuuf4vlrphecw50vgywemdd7xehh4tw</v>
       </c>
       <c r="B20">
-        <v>11.205301</v>
+        <v>6829.221888</v>
       </c>
       <c r="C20">
         <v>746610.000006</v>
@@ -865,7 +865,7 @@
         <v>stars1jhmk676u0lku94kdd03kr6dz5f5lcle7c8a6jn</v>
       </c>
       <c r="B25">
-        <v>1361.352039</v>
+        <v>1388.752039</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -905,10 +905,10 @@
         <v>stars1mqypstgwxah7mnw2dqh25g9f3qq55zg9g9650z</v>
       </c>
       <c r="B27">
-        <v>2357.721355</v>
+        <v>644.472393</v>
       </c>
       <c r="C27">
-        <v>104302.982477</v>
+        <v>104307.02145</v>
       </c>
       <c r="D27" t="str">
         <v>stars19cxgvr0dne98yu0js67tr6v2xt57q53h7fcde3qtvgathhnqt7rqgysax3</v>
@@ -945,7 +945,7 @@
         <v>stars14fj4wxrwgeclnjhsmd8muyzg674q7gymdf0kws</v>
       </c>
       <c r="B29">
-        <v>1762.342361</v>
+        <v>1216.879861</v>
       </c>
       <c r="C29">
         <v>300000</v>
@@ -965,7 +965,7 @@
         <v>stars1gzg9uxyvgdr3g0ccavecndj00z5994arlmnj07</v>
       </c>
       <c r="B30">
-        <v>1.546878</v>
+        <v>298.546878</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1065,7 +1065,7 @@
         <v>stars1njptwvkllqrmmgvl43m4pcnry3flracxqk5qh4</v>
       </c>
       <c r="B35">
-        <v>80357.921505</v>
+        <v>80362.961505</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1105,7 +1105,7 @@
         <v>stars1dhsrpfswkhjhennv40qhrr9c8saf0upvt324hw</v>
       </c>
       <c r="B37">
-        <v>8665.711525</v>
+        <v>8744.111525</v>
       </c>
       <c r="C37">
         <v>65000</v>
@@ -1225,7 +1225,7 @@
         <v>stars14yc957g6dqcvsp45l8ar2l8fnysy4y4p6fn4r3</v>
       </c>
       <c r="B43">
-        <v>9721.532379</v>
+        <v>9865.732379</v>
       </c>
       <c r="C43">
         <v>20000</v>
@@ -1245,7 +1245,7 @@
         <v>stars1xaa2hsl6ypyl74e2m0ts0d5vhlyrjqvp9c5fp2</v>
       </c>
       <c r="B44">
-        <v>2291.999126</v>
+        <v>2669.999126</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1285,7 +1285,7 @@
         <v>stars1c7ugpczm76rgejxv4pvnnsnauwzmtrp39h4xgp</v>
       </c>
       <c r="B46">
-        <v>15296.466243</v>
+        <v>30123.551377</v>
       </c>
       <c r="C46">
         <v>383265.48006</v>
@@ -1345,7 +1345,7 @@
         <v>stars1u96mt6h05v5mheyqux5t47nk0y7n9sr48nxvkr</v>
       </c>
       <c r="B49">
-        <v>1034.382571</v>
+        <v>4634.382571</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1385,10 +1385,10 @@
         <v>stars1x8s9gtdp8pp9q9k84ah6qzaeupszl88wj3y8ag</v>
       </c>
       <c r="B51">
-        <v>283.389054</v>
+        <v>0.535716</v>
       </c>
       <c r="C51">
-        <v>57000</v>
+        <v>57716</v>
       </c>
       <c r="D51" t="str">
         <v>stars1x7kcezlz3dex8x6lgum7wpuaqcw4k2m2ajggrqlnavrqgsg0rzuqaf72rh</v>
@@ -1525,7 +1525,7 @@
         <v>stars1j4y454dfhhxa4lryp58saajpynu5pdlqv4jdvj</v>
       </c>
       <c r="B58">
-        <v>150.837826</v>
+        <v>170.997826</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1665,10 +1665,10 @@
         <v>stars1c0s8csym37fyj0dlw4773vgwasxu28eh4vj985</v>
       </c>
       <c r="B65">
-        <v>52.983921</v>
+        <v>53.038586</v>
       </c>
       <c r="C65">
-        <v>12386.651799</v>
+        <v>12419.533725</v>
       </c>
       <c r="D65" t="str">
         <v>stars145tzpwh78y595us4k53cmlg2w9f80dvtasrv5f68hmnya7nhc8jqmtsryf</v>
@@ -1765,7 +1765,7 @@
         <v>stars1ghlszu0t5xzcrsesa6gkzzv80q5rgcq585hlpm</v>
       </c>
       <c r="B70">
-        <v>151.148249</v>
+        <v>371.148249</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1905,7 +1905,7 @@
         <v>stars1p34eqrfqvj6624uj5jw0ewg5s2cs06f59cys35</v>
       </c>
       <c r="B77">
-        <v>1.5</v>
+        <v>4.75</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -1985,7 +1985,7 @@
         <v>stars1qkkm73p5wlun2fmllf74e36nkl5uxw4t9gnvda</v>
       </c>
       <c r="B81">
-        <v>106.253201</v>
+        <v>34.248201</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>stars1exce33j7xrd6fmkvyzf3u0887gavdxksh2qlat</v>
       </c>
       <c r="B84">
-        <v>468.35</v>
+        <v>579.35</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2165,7 +2165,7 @@
         <v>stars10sxf3mrxlrrerym398sc7e9ps4a0678jskqrkh</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>6.4</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2185,7 +2185,7 @@
         <v>stars1mks5vfqd3lz9zumgdlpwd8zzk0m3kq3h0stk4a</v>
       </c>
       <c r="B91">
-        <v>15.810473</v>
+        <v>21.719858</v>
       </c>
       <c r="C91">
         <v>908.962008</v>

</xml_diff>

<commit_message>
Added script for filtering typeform submissions
</commit_message>
<xml_diff>
--- a/data/snapshots/3252783/xlsx/creators.xlsx
+++ b/data/snapshots/3252783/xlsx/creators.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -405,7 +405,7 @@
         <v>stars1satwv984d3s0kmvnlh4wnf0enh5xwgaq3jzfdd</v>
       </c>
       <c r="B2">
-        <v>35159.619052</v>
+        <v>37360.419052</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -425,7 +425,7 @@
         <v>stars13ajml9hrmlt2273ck5hcl5zgskk3aas2tva6fk</v>
       </c>
       <c r="B3">
-        <v>1923.499131</v>
+        <v>5550.949131</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -445,7 +445,7 @@
         <v>stars1sr7p3esz5xjsezzwrk6ec5hz2675jr692mzjul</v>
       </c>
       <c r="B4">
-        <v>1340.040996</v>
+        <v>2640.920996</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -465,7 +465,7 @@
         <v>stars154ynm3sdmprq5ete8s49l84eg66er9z586x70l</v>
       </c>
       <c r="B5">
-        <v>6709.090425</v>
+        <v>7322.390425</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -485,7 +485,7 @@
         <v>stars18q9cpwadfutwwglukawc487ed4ae40p4fkmmye</v>
       </c>
       <c r="B6">
-        <v>12140.571277</v>
+        <v>12178.146277</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -545,10 +545,10 @@
         <v>stars1d6s8v9kp4jc9qj5u9c4mrl36tss4q7ydgezre7</v>
       </c>
       <c r="B9">
-        <v>0.995319</v>
+        <v>0.960345</v>
       </c>
       <c r="C9">
-        <v>70000</v>
+        <v>70000.000001</v>
       </c>
       <c r="D9" t="str">
         <v>stars1hpgq5juh354nepq5wmwyddts3eex9t02rd4zrhqqv5nsrpht9r6sfu8v8y</v>
@@ -565,7 +565,7 @@
         <v>stars1uts2zr7lx2ln0v2rvzlx8ud2tfcya552my5h2e</v>
       </c>
       <c r="B10">
-        <v>44.70195</v>
+        <v>59.70195</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -605,7 +605,7 @@
         <v>stars1rlmqjkqtp4ctk4tw05vr08zvym7s5vyhvqpknw</v>
       </c>
       <c r="B12">
-        <v>44171.326773</v>
+        <v>44232.856773</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -645,10 +645,10 @@
         <v>stars1a67z7gyczt0npk24xpyy6ufx6l5gu546ah4l3u</v>
       </c>
       <c r="B14">
-        <v>6.260751</v>
+        <v>6.708122</v>
       </c>
       <c r="C14">
-        <v>13071.753763</v>
+        <v>13194.059996</v>
       </c>
       <c r="D14" t="str">
         <v>stars1jy9dagaycutdcjf99tp9uhl5ev9lykegp2tph6r9vu6xg3td6krs7agujy</v>
@@ -665,7 +665,7 @@
         <v>stars1zja6krwtcaa2ushn3z2m658k38qlg9qwg8casg</v>
       </c>
       <c r="B15">
-        <v>2199.204126</v>
+        <v>959.201947</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -685,7 +685,7 @@
         <v>stars1easmle9uweupe525avpzjulumcyf52y6maqysh</v>
       </c>
       <c r="B16">
-        <v>251.181764</v>
+        <v>216.199581</v>
       </c>
       <c r="C16">
         <v>50</v>
@@ -702,1567 +702,1527 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>stars1axw88ugkakle6g6ma7ev4f30lhzzyfaz3rus5u</v>
+        <v>stars1haql8s8dnn02nz5xjrwmamhskquz3aheqsjafq</v>
       </c>
       <c r="B17">
-        <v>75313.301416</v>
+        <v>52.540406</v>
       </c>
       <c r="C17">
-        <v>298329.594594</v>
+        <v>0</v>
       </c>
       <c r="D17" t="str">
-        <v>stars1ywpctek72gsccmr8gjgaamzs8vhh7ju3sjtvwk82daafavw5u0es293t0m</v>
+        <v>stars1lndsj2gufd292c35crv97ug2ncdcn9ys4s8e94wlxyeft6mt3k2svkwps9</v>
       </c>
       <c r="E17" t="str">
-        <v>ANYO Part 1</v>
+        <v>Women From Cosmos</v>
       </c>
       <c r="F17" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1ywpctek72gsccmr8gjgaamzs8vhh7ju3sjtvwk82daafavw5u0es293t0m</v>
+        <v>https://app.stargaze.zone/launchpad/stars1lndsj2gufd292c35crv97ug2ncdcn9ys4s8e94wlxyeft6mt3k2svkwps9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>stars1haql8s8dnn02nz5xjrwmamhskquz3aheqsjafq</v>
+        <v>stars19m6cng0dt0g59a2ehpcaz8zksh5u8c6seygvyn</v>
       </c>
       <c r="B18">
-        <v>203.008032</v>
+        <v>730.5</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="str">
-        <v>stars1lndsj2gufd292c35crv97ug2ncdcn9ys4s8e94wlxyeft6mt3k2svkwps9</v>
+        <v>stars14xdx2sdeergukpmjz65pt2l5n34xwn4cr8nac98d0t0583gwf6usm8w3yv</v>
       </c>
       <c r="E18" t="str">
-        <v>Women From Cosmos</v>
+        <v>Pizza</v>
       </c>
       <c r="F18" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1lndsj2gufd292c35crv97ug2ncdcn9ys4s8e94wlxyeft6mt3k2svkwps9</v>
+        <v>https://app.stargaze.zone/launchpad/stars14xdx2sdeergukpmjz65pt2l5n34xwn4cr8nac98d0t0583gwf6usm8w3yv</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>stars19m6cng0dt0g59a2ehpcaz8zksh5u8c6seygvyn</v>
+        <v>stars19kh5z7ujuuf4vlrphecw50vgywemdd7xehh4tw</v>
       </c>
       <c r="B19">
-        <v>730.5</v>
+        <v>32.126828</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>757674.000006</v>
       </c>
       <c r="D19" t="str">
-        <v>stars14xdx2sdeergukpmjz65pt2l5n34xwn4cr8nac98d0t0583gwf6usm8w3yv</v>
+        <v>stars1m95chyen8tqrawmjhxrewcwscg5vj8pkxzxeaw8em7fnjwth8rusaftwk4</v>
       </c>
       <c r="E19" t="str">
-        <v>Pizza</v>
+        <v>114Shut</v>
       </c>
       <c r="F19" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars14xdx2sdeergukpmjz65pt2l5n34xwn4cr8nac98d0t0583gwf6usm8w3yv</v>
+        <v>https://app.stargaze.zone/launchpad/stars1m95chyen8tqrawmjhxrewcwscg5vj8pkxzxeaw8em7fnjwth8rusaftwk4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>stars19kh5z7ujuuf4vlrphecw50vgywemdd7xehh4tw</v>
+        <v>stars1g5u6y4r850vsqgvex4etztqej06lxmhg2xeyc2</v>
       </c>
       <c r="B20">
-        <v>6829.221888</v>
+        <v>6222.973784</v>
       </c>
       <c r="C20">
-        <v>746610.000006</v>
+        <v>19000</v>
       </c>
       <c r="D20" t="str">
-        <v>stars1m95chyen8tqrawmjhxrewcwscg5vj8pkxzxeaw8em7fnjwth8rusaftwk4</v>
+        <v>stars1fqsqgjlurc7z2sntulfa0f9alk2ke5npyxrze9deq7lujas7m3ss7vq2fe</v>
       </c>
       <c r="E20" t="str">
-        <v>114Shut</v>
+        <v>Starty</v>
       </c>
       <c r="F20" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1m95chyen8tqrawmjhxrewcwscg5vj8pkxzxeaw8em7fnjwth8rusaftwk4</v>
+        <v>https://app.stargaze.zone/launchpad/stars1fqsqgjlurc7z2sntulfa0f9alk2ke5npyxrze9deq7lujas7m3ss7vq2fe</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>stars1g5u6y4r850vsqgvex4etztqej06lxmhg2xeyc2</v>
+        <v>stars1l2r2r5v5f8qt4ct7ahjpa93n85a2j2t39xm0wh</v>
       </c>
       <c r="B21">
-        <v>5487.609524</v>
+        <v>9.300412</v>
       </c>
       <c r="C21">
-        <v>19000</v>
+        <v>25001</v>
       </c>
       <c r="D21" t="str">
-        <v>stars1fqsqgjlurc7z2sntulfa0f9alk2ke5npyxrze9deq7lujas7m3ss7vq2fe</v>
+        <v>stars1kydlyzdwqkyxw360hu95320p62tu98mz04sk2p33as0j9pa20d6qyzhjc5</v>
       </c>
       <c r="E21" t="str">
-        <v>Starty</v>
+        <v>Army of Ra</v>
       </c>
       <c r="F21" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1fqsqgjlurc7z2sntulfa0f9alk2ke5npyxrze9deq7lujas7m3ss7vq2fe</v>
+        <v>https://app.stargaze.zone/launchpad/stars1kydlyzdwqkyxw360hu95320p62tu98mz04sk2p33as0j9pa20d6qyzhjc5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>stars1l2r2r5v5f8qt4ct7ahjpa93n85a2j2t39xm0wh</v>
+        <v>stars1wqphgxlxt5f46vyrqdgraxk2045mmlgvfzm4pk</v>
       </c>
       <c r="B22">
-        <v>100.426988</v>
+        <v>1.695554</v>
       </c>
       <c r="C22">
-        <v>25001</v>
+        <v>0</v>
       </c>
       <c r="D22" t="str">
-        <v>stars1kydlyzdwqkyxw360hu95320p62tu98mz04sk2p33as0j9pa20d6qyzhjc5</v>
+        <v>stars1y8hzen47d50ur5wx22m3zsgh7ws9u9a38wgadl8sg7k3fnd6jfns35cyeq</v>
       </c>
       <c r="E22" t="str">
-        <v>Army of Ra</v>
+        <v>25 Nights</v>
       </c>
       <c r="F22" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1kydlyzdwqkyxw360hu95320p62tu98mz04sk2p33as0j9pa20d6qyzhjc5</v>
+        <v>https://app.stargaze.zone/launchpad/stars1y8hzen47d50ur5wx22m3zsgh7ws9u9a38wgadl8sg7k3fnd6jfns35cyeq</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>stars1wqphgxlxt5f46vyrqdgraxk2045mmlgvfzm4pk</v>
+        <v>stars1ycetzdukxvf6zfgezd38h7hyzpwth7hjakc6xg</v>
       </c>
       <c r="B23">
-        <v>1.695554</v>
+        <v>49579.16199</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23" t="str">
-        <v>stars1y8hzen47d50ur5wx22m3zsgh7ws9u9a38wgadl8sg7k3fnd6jfns35cyeq</v>
+        <v>stars13uulcmq0j6cj8rve6csgcd00afg9c2wf5gqqe6kxay75c3dzrp2qumteff</v>
       </c>
       <c r="E23" t="str">
-        <v>25 Nights</v>
+        <v>Oblitus | Forgotten Worlds</v>
       </c>
       <c r="F23" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1y8hzen47d50ur5wx22m3zsgh7ws9u9a38wgadl8sg7k3fnd6jfns35cyeq</v>
+        <v>https://app.stargaze.zone/launchpad/stars13uulcmq0j6cj8rve6csgcd00afg9c2wf5gqqe6kxay75c3dzrp2qumteff</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>stars1ycetzdukxvf6zfgezd38h7hyzpwth7hjakc6xg</v>
+        <v>stars1jhmk676u0lku94kdd03kr6dz5f5lcle7c8a6jn</v>
       </c>
       <c r="B24">
-        <v>49561.32199</v>
+        <v>1866.052039</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24" t="str">
-        <v>stars13uulcmq0j6cj8rve6csgcd00afg9c2wf5gqqe6kxay75c3dzrp2qumteff</v>
+        <v>stars1uu7ggnkl4knssngtsqlnjtyy20xkln9343c7qrv6j2fj8luqr50qwm923h</v>
       </c>
       <c r="E24" t="str">
-        <v>Oblitus | Forgotten Worlds</v>
+        <v>Alpha Centaurians</v>
       </c>
       <c r="F24" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars13uulcmq0j6cj8rve6csgcd00afg9c2wf5gqqe6kxay75c3dzrp2qumteff</v>
+        <v>https://app.stargaze.zone/launchpad/stars1uu7ggnkl4knssngtsqlnjtyy20xkln9343c7qrv6j2fj8luqr50qwm923h</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>stars1jhmk676u0lku94kdd03kr6dz5f5lcle7c8a6jn</v>
+        <v>stars1uh2tythruupasd2p8x83retnqhgzyc5hzwujjq</v>
       </c>
       <c r="B25">
-        <v>1388.752039</v>
+        <v>355697.672998</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="str">
-        <v>stars1uu7ggnkl4knssngtsqlnjtyy20xkln9343c7qrv6j2fj8luqr50qwm923h</v>
+        <v>stars1t8r3w25qzpucwxw9e3s5fwqjkvn8uw3jvgvgukpzm9afehy7fmesl8ftcu</v>
       </c>
       <c r="E25" t="str">
-        <v>Alpha Centaurians</v>
+        <v>Bored Puzzles</v>
       </c>
       <c r="F25" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1uu7ggnkl4knssngtsqlnjtyy20xkln9343c7qrv6j2fj8luqr50qwm923h</v>
+        <v>https://app.stargaze.zone/launchpad/stars1t8r3w25qzpucwxw9e3s5fwqjkvn8uw3jvgvgukpzm9afehy7fmesl8ftcu</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>stars1uh2tythruupasd2p8x83retnqhgzyc5hzwujjq</v>
+        <v>stars1mqypstgwxah7mnw2dqh25g9f3qq55zg9g9650z</v>
       </c>
       <c r="B26">
-        <v>355696.672998</v>
+        <v>80861.702039</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>104321.205588</v>
       </c>
       <c r="D26" t="str">
-        <v>stars1t8r3w25qzpucwxw9e3s5fwqjkvn8uw3jvgvgukpzm9afehy7fmesl8ftcu</v>
+        <v>stars19cxgvr0dne98yu0js67tr6v2xt57q53h7fcde3qtvgathhnqt7rqgysax3</v>
       </c>
       <c r="E26" t="str">
-        <v>Bored Puzzles</v>
+        <v>The WadSquad</v>
       </c>
       <c r="F26" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1t8r3w25qzpucwxw9e3s5fwqjkvn8uw3jvgvgukpzm9afehy7fmesl8ftcu</v>
+        <v>https://app.stargaze.zone/launchpad/stars19cxgvr0dne98yu0js67tr6v2xt57q53h7fcde3qtvgathhnqt7rqgysax3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>stars1mqypstgwxah7mnw2dqh25g9f3qq55zg9g9650z</v>
+        <v>stars1fwhjk7qyfctzwrlzeqjdn53yfvw5tfvnjv4yrv</v>
       </c>
       <c r="B27">
-        <v>644.472393</v>
+        <v>933.276353</v>
       </c>
       <c r="C27">
-        <v>104307.02145</v>
+        <v>0</v>
       </c>
       <c r="D27" t="str">
-        <v>stars19cxgvr0dne98yu0js67tr6v2xt57q53h7fcde3qtvgathhnqt7rqgysax3</v>
+        <v>stars1g0tvy7kahkn4fcs7qdh7sqlu89jv3kya59n3208430egzhcrrzwq7nd2s6</v>
       </c>
       <c r="E27" t="str">
-        <v>The WadSquad</v>
+        <v>IBC Baby Apes Club</v>
       </c>
       <c r="F27" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars19cxgvr0dne98yu0js67tr6v2xt57q53h7fcde3qtvgathhnqt7rqgysax3</v>
+        <v>https://app.stargaze.zone/launchpad/stars1g0tvy7kahkn4fcs7qdh7sqlu89jv3kya59n3208430egzhcrrzwq7nd2s6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>stars1fwhjk7qyfctzwrlzeqjdn53yfvw5tfvnjv4yrv</v>
+        <v>stars14fj4wxrwgeclnjhsmd8muyzg674q7gymdf0kws</v>
       </c>
       <c r="B28">
-        <v>662.376353</v>
+        <v>3451.899177</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>310000</v>
       </c>
       <c r="D28" t="str">
-        <v>stars1g0tvy7kahkn4fcs7qdh7sqlu89jv3kya59n3208430egzhcrrzwq7nd2s6</v>
+        <v>stars1lnrdwhf4xcx6w6tdpsghgv6uavem353gtgz77sdreyhts883wdjq52aewm</v>
       </c>
       <c r="E28" t="str">
-        <v>IBC Baby Apes Club</v>
+        <v>Horizons Unbound</v>
       </c>
       <c r="F28" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1g0tvy7kahkn4fcs7qdh7sqlu89jv3kya59n3208430egzhcrrzwq7nd2s6</v>
+        <v>https://app.stargaze.zone/launchpad/stars1lnrdwhf4xcx6w6tdpsghgv6uavem353gtgz77sdreyhts883wdjq52aewm</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>stars14fj4wxrwgeclnjhsmd8muyzg674q7gymdf0kws</v>
+        <v>stars1gzg9uxyvgdr3g0ccavecndj00z5994arlmnj07</v>
       </c>
       <c r="B29">
-        <v>1216.879861</v>
+        <v>1173.132531</v>
       </c>
       <c r="C29">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="D29" t="str">
-        <v>stars1lnrdwhf4xcx6w6tdpsghgv6uavem353gtgz77sdreyhts883wdjq52aewm</v>
+        <v>stars1z6wep7u638fmyehatcyc7j7tjxl8lw4dk3jlzkq90yfxfq66vsns80v0mh</v>
       </c>
       <c r="E29" t="str">
-        <v>Horizons Unbound</v>
+        <v>Sunnyside Reapers</v>
       </c>
       <c r="F29" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1lnrdwhf4xcx6w6tdpsghgv6uavem353gtgz77sdreyhts883wdjq52aewm</v>
+        <v>https://app.stargaze.zone/launchpad/stars1z6wep7u638fmyehatcyc7j7tjxl8lw4dk3jlzkq90yfxfq66vsns80v0mh</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>stars1gzg9uxyvgdr3g0ccavecndj00z5994arlmnj07</v>
+        <v>stars1luzrdy87cjczt4nzjm2s7c2ysqe5l6nanrppsx</v>
       </c>
       <c r="B30">
-        <v>298.546878</v>
+        <v>2.50195</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30" t="str">
-        <v>stars1z6wep7u638fmyehatcyc7j7tjxl8lw4dk3jlzkq90yfxfq66vsns80v0mh</v>
+        <v>stars1l6j9z82fvpn0mzkztmjz0zu78kj9nuh68vdd6czs8tq00ngltnxq96t5d9</v>
       </c>
       <c r="E30" t="str">
-        <v>Sunnyside Reapers</v>
+        <v>Poppex</v>
       </c>
       <c r="F30" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1z6wep7u638fmyehatcyc7j7tjxl8lw4dk3jlzkq90yfxfq66vsns80v0mh</v>
+        <v>https://app.stargaze.zone/launchpad/stars1l6j9z82fvpn0mzkztmjz0zu78kj9nuh68vdd6czs8tq00ngltnxq96t5d9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>stars1luzrdy87cjczt4nzjm2s7c2ysqe5l6nanrppsx</v>
+        <v>stars1ducjvhvelvg8z4ndf23qesk0t0qk7gfuvl342f</v>
       </c>
       <c r="B31">
-        <v>1.00195</v>
+        <v>115.9</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" t="str">
-        <v>stars1l6j9z82fvpn0mzkztmjz0zu78kj9nuh68vdd6czs8tq00ngltnxq96t5d9</v>
+        <v>stars1p0shlmt62g9m300qmxn7necwag2yd8cjrvaks8z783fj6w906suqe0zz06</v>
       </c>
       <c r="E31" t="str">
-        <v>Poppex</v>
+        <v>Shnubbles Breakfast Drop</v>
       </c>
       <c r="F31" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1l6j9z82fvpn0mzkztmjz0zu78kj9nuh68vdd6czs8tq00ngltnxq96t5d9</v>
+        <v>https://app.stargaze.zone/launchpad/stars1p0shlmt62g9m300qmxn7necwag2yd8cjrvaks8z783fj6w906suqe0zz06</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>stars1ducjvhvelvg8z4ndf23qesk0t0qk7gfuvl342f</v>
+        <v>stars1h33zzkyyk4g8l3m3tjzlwjspwr96tmarc2mym9</v>
       </c>
       <c r="B32">
-        <v>115.9</v>
+        <v>1101.356477</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" t="str">
-        <v>stars1p0shlmt62g9m300qmxn7necwag2yd8cjrvaks8z783fj6w906suqe0zz06</v>
+        <v>stars194u9s4qvujm06573me7lcf5nuxj9vr690syllnrpd4w4mvpncjvs6rc2w0</v>
       </c>
       <c r="E32" t="str">
-        <v>Shnubbles Breakfast Drop</v>
+        <v>Starchoadz</v>
       </c>
       <c r="F32" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1p0shlmt62g9m300qmxn7necwag2yd8cjrvaks8z783fj6w906suqe0zz06</v>
+        <v>https://app.stargaze.zone/launchpad/stars194u9s4qvujm06573me7lcf5nuxj9vr690syllnrpd4w4mvpncjvs6rc2w0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>stars1h33zzkyyk4g8l3m3tjzlwjspwr96tmarc2mym9</v>
+        <v>stars155pp56y9u8q8pa2fc9sr2rvyvzs56tusxuxud8</v>
       </c>
       <c r="B33">
-        <v>1101.356477</v>
+        <v>378.00195</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" t="str">
-        <v>stars194u9s4qvujm06573me7lcf5nuxj9vr690syllnrpd4w4mvpncjvs6rc2w0</v>
+        <v>stars1qetvausf453rrtt8lg0lrwc3txkju9tpma5kxagua58u26wkrvfqq7h0z9</v>
       </c>
       <c r="E33" t="str">
-        <v>Starchoadz</v>
+        <v>stargaze mfers</v>
       </c>
       <c r="F33" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars194u9s4qvujm06573me7lcf5nuxj9vr690syllnrpd4w4mvpncjvs6rc2w0</v>
+        <v>https://app.stargaze.zone/launchpad/stars1qetvausf453rrtt8lg0lrwc3txkju9tpma5kxagua58u26wkrvfqq7h0z9</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>stars155pp56y9u8q8pa2fc9sr2rvyvzs56tusxuxud8</v>
+        <v>stars1njptwvkllqrmmgvl43m4pcnry3flracxqk5qh4</v>
       </c>
       <c r="B34">
-        <v>378.00195</v>
+        <v>80404.561505</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" t="str">
-        <v>stars1qetvausf453rrtt8lg0lrwc3txkju9tpma5kxagua58u26wkrvfqq7h0z9</v>
+        <v>stars1ng7e7cgftnpp5f8tkx4lfyhylt93kr5zxnqasxdywrrz2hy82jwqgp8a78</v>
       </c>
       <c r="E34" t="str">
-        <v>stargaze mfers</v>
+        <v>MultiScape</v>
       </c>
       <c r="F34" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1qetvausf453rrtt8lg0lrwc3txkju9tpma5kxagua58u26wkrvfqq7h0z9</v>
+        <v>https://app.stargaze.zone/launchpad/stars1ng7e7cgftnpp5f8tkx4lfyhylt93kr5zxnqasxdywrrz2hy82jwqgp8a78</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>stars1njptwvkllqrmmgvl43m4pcnry3flracxqk5qh4</v>
+        <v>stars1z3tyff59d3hlptwjyxxlp86k68f7w5mfrc083q</v>
       </c>
       <c r="B35">
-        <v>80362.961505</v>
+        <v>11.709352</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1666.592173</v>
       </c>
       <c r="D35" t="str">
-        <v>stars1ng7e7cgftnpp5f8tkx4lfyhylt93kr5zxnqasxdywrrz2hy82jwqgp8a78</v>
+        <v>stars1ua9rnvdv7sd4tkdsmjgl8v32mw8465s4d5v4fwskqdr8ahlp0nuq4g8tkl</v>
       </c>
       <c r="E35" t="str">
-        <v>MultiScape</v>
+        <v>StarGazed Flwrs</v>
       </c>
       <c r="F35" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1ng7e7cgftnpp5f8tkx4lfyhylt93kr5zxnqasxdywrrz2hy82jwqgp8a78</v>
+        <v>https://app.stargaze.zone/launchpad/stars1ua9rnvdv7sd4tkdsmjgl8v32mw8465s4d5v4fwskqdr8ahlp0nuq4g8tkl</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>stars1z3tyff59d3hlptwjyxxlp86k68f7w5mfrc083q</v>
+        <v>stars1dhsrpfswkhjhennv40qhrr9c8saf0upvt324hw</v>
       </c>
       <c r="B36">
-        <v>11.709352</v>
+        <v>10284.993398</v>
       </c>
       <c r="C36">
-        <v>1666.592173</v>
+        <v>65000</v>
       </c>
       <c r="D36" t="str">
-        <v>stars1ua9rnvdv7sd4tkdsmjgl8v32mw8465s4d5v4fwskqdr8ahlp0nuq4g8tkl</v>
+        <v>stars1gx87aqhck908zttzkms7wpgs3d6ljeg2nzh9kz2vwp326vp5pslqdjxhde</v>
       </c>
       <c r="E36" t="str">
-        <v>StarGazed Flwrs</v>
+        <v>C∅smoVoyagers</v>
       </c>
       <c r="F36" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1ua9rnvdv7sd4tkdsmjgl8v32mw8465s4d5v4fwskqdr8ahlp0nuq4g8tkl</v>
+        <v>https://app.stargaze.zone/launchpad/stars1gx87aqhck908zttzkms7wpgs3d6ljeg2nzh9kz2vwp326vp5pslqdjxhde</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>stars1dhsrpfswkhjhennv40qhrr9c8saf0upvt324hw</v>
+        <v>stars17tejgfxsc73qxecjk3sy0jfujrn9d2tj2yt7n4</v>
       </c>
       <c r="B37">
-        <v>8744.111525</v>
+        <v>71.28508</v>
       </c>
       <c r="C37">
-        <v>65000</v>
+        <v>0</v>
       </c>
       <c r="D37" t="str">
-        <v>stars1gx87aqhck908zttzkms7wpgs3d6ljeg2nzh9kz2vwp326vp5pslqdjxhde</v>
+        <v>stars1ljjghtxmv93sdhfawlm7ewudgfpsne50pxh35ldys944g2qtlgsqk2ysqs</v>
       </c>
       <c r="E37" t="str">
-        <v>C∅smoVoyagers</v>
+        <v>Cute Crypto Girls SG</v>
       </c>
       <c r="F37" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1gx87aqhck908zttzkms7wpgs3d6ljeg2nzh9kz2vwp326vp5pslqdjxhde</v>
+        <v>https://app.stargaze.zone/launchpad/stars1ljjghtxmv93sdhfawlm7ewudgfpsne50pxh35ldys944g2qtlgsqk2ysqs</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>stars17tejgfxsc73qxecjk3sy0jfujrn9d2tj2yt7n4</v>
+        <v>stars13gl70rqxqjzygqancjqzu486xxdvgmjtjd7sul</v>
       </c>
       <c r="B38">
-        <v>71.28508</v>
+        <v>6999.999772</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38" t="str">
-        <v>stars1ljjghtxmv93sdhfawlm7ewudgfpsne50pxh35ldys944g2qtlgsqk2ysqs</v>
+        <v>stars1zwn7j7hfddk2yz66q4ddw2lqw35qlaqxnkdwg79pqhje5dv83m4stzxdax</v>
       </c>
       <c r="E38" t="str">
-        <v>Cute Crypto Girls SG</v>
+        <v>Andromaverse</v>
       </c>
       <c r="F38" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1ljjghtxmv93sdhfawlm7ewudgfpsne50pxh35ldys944g2qtlgsqk2ysqs</v>
+        <v>https://app.stargaze.zone/launchpad/stars1zwn7j7hfddk2yz66q4ddw2lqw35qlaqxnkdwg79pqhje5dv83m4stzxdax</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>stars13gl70rqxqjzygqancjqzu486xxdvgmjtjd7sul</v>
+        <v>stars1jfkxx25wqkp7dt6jx2a756lw3f9v29rqgqwpkc</v>
       </c>
       <c r="B39">
-        <v>2.896638</v>
+        <v>0.100458</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>5909.108748</v>
       </c>
       <c r="D39" t="str">
-        <v>stars1zwn7j7hfddk2yz66q4ddw2lqw35qlaqxnkdwg79pqhje5dv83m4stzxdax</v>
+        <v>stars1sxvt8j79sqdf5nwnltga77u7emsyqxzv0wlpwnxjfvej0yetzyqsxr96qy</v>
       </c>
       <c r="E39" t="str">
-        <v>Andromaverse</v>
+        <v>AI Artist Samoyed Ash Collection</v>
       </c>
       <c r="F39" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1zwn7j7hfddk2yz66q4ddw2lqw35qlaqxnkdwg79pqhje5dv83m4stzxdax</v>
+        <v>https://app.stargaze.zone/launchpad/stars1sxvt8j79sqdf5nwnltga77u7emsyqxzv0wlpwnxjfvej0yetzyqsxr96qy</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>stars1jfkxx25wqkp7dt6jx2a756lw3f9v29rqgqwpkc</v>
+        <v>stars1xpcghcmf6eex3hzru8y4wnu8eu8z6elqplscqu</v>
       </c>
       <c r="B40">
-        <v>0.100458</v>
+        <v>0.00195</v>
       </c>
       <c r="C40">
-        <v>5909.108748</v>
+        <v>76904.931078</v>
       </c>
       <c r="D40" t="str">
-        <v>stars1sxvt8j79sqdf5nwnltga77u7emsyqxzv0wlpwnxjfvej0yetzyqsxr96qy</v>
+        <v>stars1cnpp5lclzeegm2rjtrxha875cqjnuz370yytuxltlugdwwc6m4nsay8xkw</v>
       </c>
       <c r="E40" t="str">
-        <v>AI Artist Samoyed Ash Collection</v>
+        <v>Happy Puppies</v>
       </c>
       <c r="F40" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1sxvt8j79sqdf5nwnltga77u7emsyqxzv0wlpwnxjfvej0yetzyqsxr96qy</v>
+        <v>https://app.stargaze.zone/launchpad/stars1cnpp5lclzeegm2rjtrxha875cqjnuz370yytuxltlugdwwc6m4nsay8xkw</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>stars1xpcghcmf6eex3hzru8y4wnu8eu8z6elqplscqu</v>
+        <v>stars1rvu4yapuyvk0x3hcua7ntz9nn8h2505ajvf3kz</v>
       </c>
       <c r="B41">
-        <v>0.00195</v>
+        <v>177.497831</v>
       </c>
       <c r="C41">
-        <v>76904.931078</v>
+        <v>0</v>
       </c>
       <c r="D41" t="str">
-        <v>stars1cnpp5lclzeegm2rjtrxha875cqjnuz370yytuxltlugdwwc6m4nsay8xkw</v>
+        <v>stars1klg9pj576qra5862svgwcs07r40sdks4xk62j3t9567k2z79nr6qn406kq</v>
       </c>
       <c r="E41" t="str">
-        <v>Happy Puppies</v>
+        <v>Classified Cats</v>
       </c>
       <c r="F41" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1cnpp5lclzeegm2rjtrxha875cqjnuz370yytuxltlugdwwc6m4nsay8xkw</v>
+        <v>https://app.stargaze.zone/launchpad/stars1klg9pj576qra5862svgwcs07r40sdks4xk62j3t9567k2z79nr6qn406kq</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>stars1rvu4yapuyvk0x3hcua7ntz9nn8h2505ajvf3kz</v>
+        <v>stars14yc957g6dqcvsp45l8ar2l8fnysy4y4p6fn4r3</v>
       </c>
       <c r="B42">
-        <v>177.497831</v>
+        <v>10501.268775</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="D42" t="str">
-        <v>stars1klg9pj576qra5862svgwcs07r40sdks4xk62j3t9567k2z79nr6qn406kq</v>
+        <v>stars1nx6l8x7kr8h5z4nvmaru264jg4rfqf0eceznfgmhyhghge4v7k5sdhey8q</v>
       </c>
       <c r="E42" t="str">
-        <v>Classified Cats</v>
+        <v>Stargazers - First Federation</v>
       </c>
       <c r="F42" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1klg9pj576qra5862svgwcs07r40sdks4xk62j3t9567k2z79nr6qn406kq</v>
+        <v>https://app.stargaze.zone/launchpad/stars1nx6l8x7kr8h5z4nvmaru264jg4rfqf0eceznfgmhyhghge4v7k5sdhey8q</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>stars14yc957g6dqcvsp45l8ar2l8fnysy4y4p6fn4r3</v>
+        <v>stars1xaa2hsl6ypyl74e2m0ts0d5vhlyrjqvp9c5fp2</v>
       </c>
       <c r="B43">
-        <v>9865.732379</v>
+        <v>3803.999126</v>
       </c>
       <c r="C43">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="D43" t="str">
-        <v>stars1nx6l8x7kr8h5z4nvmaru264jg4rfqf0eceznfgmhyhghge4v7k5sdhey8q</v>
+        <v>stars1cpzvvmlrc9lcw3q5yrznax0uk5h6xww2d4ch9xve4xu8mfvgw2kqepnwd2</v>
       </c>
       <c r="E43" t="str">
-        <v>Stargazers - First Federation</v>
+        <v>BitCanna Buddheads</v>
       </c>
       <c r="F43" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1nx6l8x7kr8h5z4nvmaru264jg4rfqf0eceznfgmhyhghge4v7k5sdhey8q</v>
+        <v>https://app.stargaze.zone/launchpad/stars1cpzvvmlrc9lcw3q5yrznax0uk5h6xww2d4ch9xve4xu8mfvgw2kqepnwd2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>stars1xaa2hsl6ypyl74e2m0ts0d5vhlyrjqvp9c5fp2</v>
+        <v>stars1q0j47saq9xun853n92kj89098tnfqhtcu64h3k</v>
       </c>
       <c r="B44">
-        <v>2669.999126</v>
+        <v>810.00195</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44" t="str">
-        <v>stars1cpzvvmlrc9lcw3q5yrznax0uk5h6xww2d4ch9xve4xu8mfvgw2kqepnwd2</v>
+        <v>stars1u0xl257qeqt9ltrtn3wnwrxjtv8qvkhemxcswj4f9km7n0tqvn7q5zxnvu</v>
       </c>
       <c r="E44" t="str">
-        <v>BitCanna Buddheads</v>
+        <v>starstudents</v>
       </c>
       <c r="F44" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1cpzvvmlrc9lcw3q5yrznax0uk5h6xww2d4ch9xve4xu8mfvgw2kqepnwd2</v>
+        <v>https://app.stargaze.zone/launchpad/stars1u0xl257qeqt9ltrtn3wnwrxjtv8qvkhemxcswj4f9km7n0tqvn7q5zxnvu</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>stars1q0j47saq9xun853n92kj89098tnfqhtcu64h3k</v>
+        <v>stars1c7ugpczm76rgejxv4pvnnsnauwzmtrp39h4xgp</v>
       </c>
       <c r="B45">
-        <v>810.00195</v>
+        <v>31112.8728</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>383265.48006</v>
       </c>
       <c r="D45" t="str">
-        <v>stars1u0xl257qeqt9ltrtn3wnwrxjtv8qvkhemxcswj4f9km7n0tqvn7q5zxnvu</v>
+        <v>stars1c6khwcyaku4rd08tg7rg33h8rx9d9g0p679hk2aw6arynj79mhyqx94p0q</v>
       </c>
       <c r="E45" t="str">
-        <v>starstudents</v>
+        <v>RePop</v>
       </c>
       <c r="F45" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1u0xl257qeqt9ltrtn3wnwrxjtv8qvkhemxcswj4f9km7n0tqvn7q5zxnvu</v>
+        <v>https://app.stargaze.zone/launchpad/stars1c6khwcyaku4rd08tg7rg33h8rx9d9g0p679hk2aw6arynj79mhyqx94p0q</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>stars1c7ugpczm76rgejxv4pvnnsnauwzmtrp39h4xgp</v>
+        <v>stars182qekjkz45pjmr5070v4qdlaxfxqeu3alqcyvx</v>
       </c>
       <c r="B46">
-        <v>30123.551377</v>
+        <v>2.969459</v>
       </c>
       <c r="C46">
-        <v>383265.48006</v>
+        <v>0</v>
       </c>
       <c r="D46" t="str">
-        <v>stars1c6khwcyaku4rd08tg7rg33h8rx9d9g0p679hk2aw6arynj79mhyqx94p0q</v>
+        <v>stars1c7hrh6q2530m4m4ll72vds4j766fuphdqw20ayp4p23npr46hczs6th2kf</v>
       </c>
       <c r="E46" t="str">
-        <v>RePop</v>
+        <v>Stargaze Miners</v>
       </c>
       <c r="F46" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1c6khwcyaku4rd08tg7rg33h8rx9d9g0p679hk2aw6arynj79mhyqx94p0q</v>
+        <v>https://app.stargaze.zone/launchpad/stars1c7hrh6q2530m4m4ll72vds4j766fuphdqw20ayp4p23npr46hczs6th2kf</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>stars182qekjkz45pjmr5070v4qdlaxfxqeu3alqcyvx</v>
+        <v>stars1hq09acf87at9vg9pg9ruzup2fsp2400dh6u2rh</v>
       </c>
       <c r="B47">
-        <v>522.972709</v>
+        <v>44.102133</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1001</v>
       </c>
       <c r="D47" t="str">
-        <v>stars1c7hrh6q2530m4m4ll72vds4j766fuphdqw20ayp4p23npr46hczs6th2kf</v>
+        <v>stars1m2276mc8mzmzta228a9ymlv9ev83v0pu6a9v8n5l0jtg47w06n2qpd4kz5</v>
       </c>
       <c r="E47" t="str">
-        <v>Stargaze Miners</v>
+        <v>Crazy Doodle NFT</v>
       </c>
       <c r="F47" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1c7hrh6q2530m4m4ll72vds4j766fuphdqw20ayp4p23npr46hczs6th2kf</v>
+        <v>https://app.stargaze.zone/launchpad/stars1m2276mc8mzmzta228a9ymlv9ev83v0pu6a9v8n5l0jtg47w06n2qpd4kz5</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>stars1hq09acf87at9vg9pg9ruzup2fsp2400dh6u2rh</v>
+        <v>stars1u96mt6h05v5mheyqux5t47nk0y7n9sr48nxvkr</v>
       </c>
       <c r="B48">
-        <v>44.102133</v>
+        <v>12998.032571</v>
       </c>
       <c r="C48">
-        <v>1001</v>
+        <v>0</v>
       </c>
       <c r="D48" t="str">
-        <v>stars1m2276mc8mzmzta228a9ymlv9ev83v0pu6a9v8n5l0jtg47w06n2qpd4kz5</v>
+        <v>stars1ey26a07wzh3kd3vekn7dn3kp4z2n7xddxncnh03tn6ha83ft3l6qt5szh4</v>
       </c>
       <c r="E48" t="str">
-        <v>Crazy Doodle NFT</v>
+        <v>War Cats</v>
       </c>
       <c r="F48" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1m2276mc8mzmzta228a9ymlv9ev83v0pu6a9v8n5l0jtg47w06n2qpd4kz5</v>
+        <v>https://app.stargaze.zone/launchpad/stars1ey26a07wzh3kd3vekn7dn3kp4z2n7xddxncnh03tn6ha83ft3l6qt5szh4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>stars1u96mt6h05v5mheyqux5t47nk0y7n9sr48nxvkr</v>
+        <v>stars15z3rrky9jvk33mpjkd63z9sc2tfm7z0xq50spx</v>
       </c>
       <c r="B49">
-        <v>4634.382571</v>
+        <v>38.206789</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D49" t="str">
-        <v>stars1ey26a07wzh3kd3vekn7dn3kp4z2n7xddxncnh03tn6ha83ft3l6qt5szh4</v>
+        <v>stars1ywlmr92mxwj6c45h7snumffv59arld6c3cnnljcqxh0h4652eansdx3j2p</v>
       </c>
       <c r="E49" t="str">
-        <v>War Cats</v>
+        <v>Star Equinox</v>
       </c>
       <c r="F49" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1ey26a07wzh3kd3vekn7dn3kp4z2n7xddxncnh03tn6ha83ft3l6qt5szh4</v>
+        <v>https://app.stargaze.zone/launchpad/stars1ywlmr92mxwj6c45h7snumffv59arld6c3cnnljcqxh0h4652eansdx3j2p</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>stars15z3rrky9jvk33mpjkd63z9sc2tfm7z0xq50spx</v>
+        <v>stars1x8s9gtdp8pp9q9k84ah6qzaeupszl88wj3y8ag</v>
       </c>
       <c r="B50">
-        <v>129.610356</v>
+        <v>0.535716</v>
       </c>
       <c r="C50">
-        <v>1000</v>
+        <v>57716</v>
       </c>
       <c r="D50" t="str">
-        <v>stars1ywlmr92mxwj6c45h7snumffv59arld6c3cnnljcqxh0h4652eansdx3j2p</v>
+        <v>stars1x7kcezlz3dex8x6lgum7wpuaqcw4k2m2ajggrqlnavrqgsg0rzuqaf72rh</v>
       </c>
       <c r="E50" t="str">
-        <v>Star Equinox</v>
+        <v>Waifu</v>
       </c>
       <c r="F50" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1ywlmr92mxwj6c45h7snumffv59arld6c3cnnljcqxh0h4652eansdx3j2p</v>
+        <v>https://app.stargaze.zone/launchpad/stars1x7kcezlz3dex8x6lgum7wpuaqcw4k2m2ajggrqlnavrqgsg0rzuqaf72rh</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>stars1x8s9gtdp8pp9q9k84ah6qzaeupszl88wj3y8ag</v>
+        <v>stars1w09l7fclqyzvkvflncezrsexh0knmk7m469ae8</v>
       </c>
       <c r="B51">
-        <v>0.535716</v>
+        <v>9.959998</v>
       </c>
       <c r="C51">
-        <v>57716</v>
+        <v>0</v>
       </c>
       <c r="D51" t="str">
-        <v>stars1x7kcezlz3dex8x6lgum7wpuaqcw4k2m2ajggrqlnavrqgsg0rzuqaf72rh</v>
+        <v>stars172gt9a6rkg7cdgc4c9vcalxy7gkyttsjvzectatmeadjdslxvm8sugxrgx</v>
       </c>
       <c r="E51" t="str">
-        <v>Waifu</v>
+        <v>Blood Ritual</v>
       </c>
       <c r="F51" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1x7kcezlz3dex8x6lgum7wpuaqcw4k2m2ajggrqlnavrqgsg0rzuqaf72rh</v>
+        <v>https://app.stargaze.zone/launchpad/stars172gt9a6rkg7cdgc4c9vcalxy7gkyttsjvzectatmeadjdslxvm8sugxrgx</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>stars1w09l7fclqyzvkvflncezrsexh0knmk7m469ae8</v>
+        <v>stars1j4t9sg9f985397k9v09z9m2k4zq70nyyyuwhcu</v>
       </c>
       <c r="B52">
-        <v>9.959998</v>
+        <v>493.466484</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52" t="str">
-        <v>stars172gt9a6rkg7cdgc4c9vcalxy7gkyttsjvzectatmeadjdslxvm8sugxrgx</v>
+        <v>stars1849ymg8edecxr95jlqdng5q2y0klnl49ua3rsdtj837h62k4pjrqge3r73</v>
       </c>
       <c r="E52" t="str">
-        <v>Blood Ritual</v>
+        <v>Wanderers</v>
       </c>
       <c r="F52" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars172gt9a6rkg7cdgc4c9vcalxy7gkyttsjvzectatmeadjdslxvm8sugxrgx</v>
+        <v>https://app.stargaze.zone/launchpad/stars1849ymg8edecxr95jlqdng5q2y0klnl49ua3rsdtj837h62k4pjrqge3r73</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>stars1j4t9sg9f985397k9v09z9m2k4zq70nyyyuwhcu</v>
+        <v>stars1hsyn58377tvqk874jhtr87pc5kdv8pz5fnj795</v>
       </c>
       <c r="B53">
-        <v>493.466484</v>
+        <v>6.284396</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>9372.642839</v>
       </c>
       <c r="D53" t="str">
-        <v>stars1849ymg8edecxr95jlqdng5q2y0klnl49ua3rsdtj837h62k4pjrqge3r73</v>
+        <v>stars1wqk4wsk0t00uu39wl96m0myky2wufvgfzcqjuusnq0q9k7zumpeq4hz9xk</v>
       </c>
       <c r="E53" t="str">
-        <v>Wanderers</v>
+        <v>Ramenheads</v>
       </c>
       <c r="F53" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1849ymg8edecxr95jlqdng5q2y0klnl49ua3rsdtj837h62k4pjrqge3r73</v>
+        <v>https://app.stargaze.zone/launchpad/stars1wqk4wsk0t00uu39wl96m0myky2wufvgfzcqjuusnq0q9k7zumpeq4hz9xk</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>stars1hsyn58377tvqk874jhtr87pc5kdv8pz5fnj795</v>
+        <v>stars1nsqeha6e6kncfw0f4yqmu5ycwedaxl8m0zexpz</v>
       </c>
       <c r="B54">
-        <v>6.284396</v>
+        <v>120.040249</v>
       </c>
       <c r="C54">
-        <v>9372.642839</v>
+        <v>0</v>
       </c>
       <c r="D54" t="str">
-        <v>stars1wqk4wsk0t00uu39wl96m0myky2wufvgfzcqjuusnq0q9k7zumpeq4hz9xk</v>
+        <v>stars1xxu093mj5mqk26h3mgjzaykyetdpl337zp34plv44xvdlreckmmqzeqwtm</v>
       </c>
       <c r="E54" t="str">
-        <v>Ramenheads</v>
+        <v>Interchain NFTs</v>
       </c>
       <c r="F54" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1wqk4wsk0t00uu39wl96m0myky2wufvgfzcqjuusnq0q9k7zumpeq4hz9xk</v>
+        <v>https://app.stargaze.zone/launchpad/stars1xxu093mj5mqk26h3mgjzaykyetdpl337zp34plv44xvdlreckmmqzeqwtm</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>stars1nsqeha6e6kncfw0f4yqmu5ycwedaxl8m0zexpz</v>
+        <v>stars1w7lfuja7faml0kgwdk33wwgcsx7ym5vc7jddl9</v>
       </c>
       <c r="B55">
-        <v>120.040249</v>
+        <v>1597.801111</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>26000</v>
       </c>
       <c r="D55" t="str">
-        <v>stars1xxu093mj5mqk26h3mgjzaykyetdpl337zp34plv44xvdlreckmmqzeqwtm</v>
+        <v>stars18tj7yvh7qxv29wtr4angy4gqycrrj9e5j9susaes7vd4tqafzthq5h2m8r</v>
       </c>
       <c r="E55" t="str">
-        <v>Interchain NFTs</v>
+        <v>Waving Cosmonauts</v>
       </c>
       <c r="F55" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1xxu093mj5mqk26h3mgjzaykyetdpl337zp34plv44xvdlreckmmqzeqwtm</v>
+        <v>https://app.stargaze.zone/launchpad/stars18tj7yvh7qxv29wtr4angy4gqycrrj9e5j9susaes7vd4tqafzthq5h2m8r</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>stars1w7lfuja7faml0kgwdk33wwgcsx7ym5vc7jddl9</v>
+        <v>stars1znmlka3nvzu0vtn05qm03qllhnx76vwnatjchr</v>
       </c>
       <c r="B56">
-        <v>1561.321111</v>
+        <v>650.75195</v>
       </c>
       <c r="C56">
-        <v>26000</v>
+        <v>0</v>
       </c>
       <c r="D56" t="str">
-        <v>stars18tj7yvh7qxv29wtr4angy4gqycrrj9e5j9susaes7vd4tqafzthq5h2m8r</v>
+        <v>stars1n0sfcgf9nu7tq4hr423dgpvy9kz67xfvd9v96u2e5cjywx7s0ymqhtucfs</v>
       </c>
       <c r="E56" t="str">
-        <v>Waving Cosmonauts</v>
+        <v>Existing</v>
       </c>
       <c r="F56" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars18tj7yvh7qxv29wtr4angy4gqycrrj9e5j9susaes7vd4tqafzthq5h2m8r</v>
+        <v>https://app.stargaze.zone/launchpad/stars1n0sfcgf9nu7tq4hr423dgpvy9kz67xfvd9v96u2e5cjywx7s0ymqhtucfs</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>stars1znmlka3nvzu0vtn05qm03qllhnx76vwnatjchr</v>
+        <v>stars1j4y454dfhhxa4lryp58saajpynu5pdlqv4jdvj</v>
       </c>
       <c r="B57">
-        <v>650.75195</v>
+        <v>79.117826</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57" t="str">
-        <v>stars1n0sfcgf9nu7tq4hr423dgpvy9kz67xfvd9v96u2e5cjywx7s0ymqhtucfs</v>
+        <v>stars1dg6tgwxhjqg6rnrf77t8ly8wcqm394q3kvuq92plk679h5jg0kasc6f9xu</v>
       </c>
       <c r="E57" t="str">
-        <v>Existing</v>
+        <v>OG Starz Club</v>
       </c>
       <c r="F57" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1n0sfcgf9nu7tq4hr423dgpvy9kz67xfvd9v96u2e5cjywx7s0ymqhtucfs</v>
+        <v>https://app.stargaze.zone/launchpad/stars1dg6tgwxhjqg6rnrf77t8ly8wcqm394q3kvuq92plk679h5jg0kasc6f9xu</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>stars1j4y454dfhhxa4lryp58saajpynu5pdlqv4jdvj</v>
+        <v>stars1cy7fszjpp8675hfqpygc4j6t0sesefmukczc2t</v>
       </c>
       <c r="B58">
-        <v>170.997826</v>
+        <v>535.45675</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58" t="str">
-        <v>stars1dg6tgwxhjqg6rnrf77t8ly8wcqm394q3kvuq92plk679h5jg0kasc6f9xu</v>
+        <v>stars1l3hnxxgw8kmxu232hdhwk5xyufxer7xvplus95xuk5904tq9n6cs3y9nck</v>
       </c>
       <c r="E58" t="str">
-        <v>OG Starz Club</v>
+        <v>AInime Girls</v>
       </c>
       <c r="F58" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1dg6tgwxhjqg6rnrf77t8ly8wcqm394q3kvuq92plk679h5jg0kasc6f9xu</v>
+        <v>https://app.stargaze.zone/launchpad/stars1l3hnxxgw8kmxu232hdhwk5xyufxer7xvplus95xuk5904tq9n6cs3y9nck</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>stars1cy7fszjpp8675hfqpygc4j6t0sesefmukczc2t</v>
+        <v>stars1rrhuws8zepv05dyc3la7wxsj56khqzpflvvmy9</v>
       </c>
       <c r="B59">
-        <v>465.45675</v>
+        <v>35.171055</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59" t="str">
-        <v>stars1l3hnxxgw8kmxu232hdhwk5xyufxer7xvplus95xuk5904tq9n6cs3y9nck</v>
+        <v>stars12a9wtxjpy78an624gfnzkz7zsphkuv2vqj95at4y8nf4auw77jys4zh7mh</v>
       </c>
       <c r="E59" t="str">
-        <v>AInime Girls</v>
+        <v>Fractalosis</v>
       </c>
       <c r="F59" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1l3hnxxgw8kmxu232hdhwk5xyufxer7xvplus95xuk5904tq9n6cs3y9nck</v>
+        <v>https://app.stargaze.zone/launchpad/stars12a9wtxjpy78an624gfnzkz7zsphkuv2vqj95at4y8nf4auw77jys4zh7mh</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>stars1rrhuws8zepv05dyc3la7wxsj56khqzpflvvmy9</v>
+        <v>stars1yxe5aj8v8tmumehtt9jd44q90zt8mvr8j5qf2p</v>
       </c>
       <c r="B60">
-        <v>35.171055</v>
+        <v>50.908798</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="D60" t="str">
-        <v>stars12a9wtxjpy78an624gfnzkz7zsphkuv2vqj95at4y8nf4auw77jys4zh7mh</v>
+        <v>stars1seg7y9m9h0f8vmx6wmhy0d2jpr2xpp2udz0m6hls6h0d62eewwzq4kalcu</v>
       </c>
       <c r="E60" t="str">
-        <v>Fractalosis</v>
+        <v>Boring Robots</v>
       </c>
       <c r="F60" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars12a9wtxjpy78an624gfnzkz7zsphkuv2vqj95at4y8nf4auw77jys4zh7mh</v>
+        <v>https://app.stargaze.zone/launchpad/stars1seg7y9m9h0f8vmx6wmhy0d2jpr2xpp2udz0m6hls6h0d62eewwzq4kalcu</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>stars1yxe5aj8v8tmumehtt9jd44q90zt8mvr8j5qf2p</v>
+        <v>stars15g509s7h5k5zwlj2tmpx0dcrt9l245kkrar30r</v>
       </c>
       <c r="B61">
-        <v>50.908798</v>
+        <v>37.62891</v>
       </c>
       <c r="C61">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="D61" t="str">
-        <v>stars1seg7y9m9h0f8vmx6wmhy0d2jpr2xpp2udz0m6hls6h0d62eewwzq4kalcu</v>
+        <v>stars1gwx369dmcw70wsmvv3zvzfr9f9hn2gszshahty9llm7z8648jprqpkrtfy</v>
       </c>
       <c r="E61" t="str">
-        <v>Boring Robots</v>
+        <v>Genesis First Press Owlies</v>
       </c>
       <c r="F61" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1seg7y9m9h0f8vmx6wmhy0d2jpr2xpp2udz0m6hls6h0d62eewwzq4kalcu</v>
+        <v>https://app.stargaze.zone/launchpad/stars1gwx369dmcw70wsmvv3zvzfr9f9hn2gszshahty9llm7z8648jprqpkrtfy</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>stars15g509s7h5k5zwlj2tmpx0dcrt9l245kkrar30r</v>
+        <v>stars1vtw4dl88vnrlws8cgnv8637x96dvkgtshq3pgk</v>
       </c>
       <c r="B62">
-        <v>41.549166</v>
+        <v>146.894577</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62" t="str">
-        <v>stars1gwx369dmcw70wsmvv3zvzfr9f9hn2gszshahty9llm7z8648jprqpkrtfy</v>
+        <v>stars1htuadyferskhuagmj0twp3tn7f65x4yh2a4t63lwcfkkasv97y0qt4psfj</v>
       </c>
       <c r="E62" t="str">
-        <v>Genesis First Press Owlies</v>
+        <v>IBC Monkes</v>
       </c>
       <c r="F62" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1gwx369dmcw70wsmvv3zvzfr9f9hn2gszshahty9llm7z8648jprqpkrtfy</v>
+        <v>https://app.stargaze.zone/launchpad/stars1htuadyferskhuagmj0twp3tn7f65x4yh2a4t63lwcfkkasv97y0qt4psfj</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>stars1vtw4dl88vnrlws8cgnv8637x96dvkgtshq3pgk</v>
+        <v>stars16rj9wa02csuhmcjluz0wu24t5s4ehkan98ja20</v>
       </c>
       <c r="B63">
-        <v>146.894577</v>
+        <v>26.533324</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63" t="str">
-        <v>stars1htuadyferskhuagmj0twp3tn7f65x4yh2a4t63lwcfkkasv97y0qt4psfj</v>
+        <v>stars1kx62tnequ4eh4c3jp9pd558h5ylkycwg6gajdyq74enrrpzw535st94xjg</v>
       </c>
       <c r="E63" t="str">
-        <v>IBC Monkes</v>
+        <v>Cosmos Ball 777</v>
       </c>
       <c r="F63" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1htuadyferskhuagmj0twp3tn7f65x4yh2a4t63lwcfkkasv97y0qt4psfj</v>
+        <v>https://app.stargaze.zone/launchpad/stars1kx62tnequ4eh4c3jp9pd558h5ylkycwg6gajdyq74enrrpzw535st94xjg</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>stars16rj9wa02csuhmcjluz0wu24t5s4ehkan98ja20</v>
+        <v>stars1c0s8csym37fyj0dlw4773vgwasxu28eh4vj985</v>
       </c>
       <c r="B64">
-        <v>26.533324</v>
+        <v>53.81261</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>12508.749276</v>
       </c>
       <c r="D64" t="str">
-        <v>stars1kx62tnequ4eh4c3jp9pd558h5ylkycwg6gajdyq74enrrpzw535st94xjg</v>
+        <v>stars145tzpwh78y595us4k53cmlg2w9f80dvtasrv5f68hmnya7nhc8jqmtsryf</v>
       </c>
       <c r="E64" t="str">
-        <v>Cosmos Ball 777</v>
+        <v>Sloth &amp; Bear Cosmos Adventure</v>
       </c>
       <c r="F64" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1kx62tnequ4eh4c3jp9pd558h5ylkycwg6gajdyq74enrrpzw535st94xjg</v>
+        <v>https://app.stargaze.zone/launchpad/stars145tzpwh78y595us4k53cmlg2w9f80dvtasrv5f68hmnya7nhc8jqmtsryf</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>stars1c0s8csym37fyj0dlw4773vgwasxu28eh4vj985</v>
+        <v>stars1aucmnevas6xd4hzdxyea3as6tqaj5dvhj8s9fx</v>
       </c>
       <c r="B65">
-        <v>53.038586</v>
+        <v>202.911999</v>
       </c>
       <c r="C65">
-        <v>12419.533725</v>
+        <v>0</v>
       </c>
       <c r="D65" t="str">
-        <v>stars145tzpwh78y595us4k53cmlg2w9f80dvtasrv5f68hmnya7nhc8jqmtsryf</v>
+        <v>stars1u5hgykavd7g5nlzgfqhyrt38a74z7t2wufymy4z20fsjjacp6v3s33kqz4</v>
       </c>
       <c r="E65" t="str">
-        <v>Sloth &amp; Bear Cosmos Adventure</v>
+        <v>SadPugs</v>
       </c>
       <c r="F65" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars145tzpwh78y595us4k53cmlg2w9f80dvtasrv5f68hmnya7nhc8jqmtsryf</v>
+        <v>https://app.stargaze.zone/launchpad/stars1u5hgykavd7g5nlzgfqhyrt38a74z7t2wufymy4z20fsjjacp6v3s33kqz4</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>stars1aucmnevas6xd4hzdxyea3as6tqaj5dvhj8s9fx</v>
+        <v>stars1kccw8qqpzkj5jcfyh72pycxs2xjfn3r2aa66xg</v>
       </c>
       <c r="B66">
-        <v>202.911999</v>
+        <v>7</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66" t="str">
-        <v>stars1u5hgykavd7g5nlzgfqhyrt38a74z7t2wufymy4z20fsjjacp6v3s33kqz4</v>
+        <v>stars1y7ev7hlvtt6jyhrz3c9zgn760yxhm2hhfnvwl52c85h2e39dn25qr2p5fm</v>
       </c>
       <c r="E66" t="str">
-        <v>SadPugs</v>
+        <v>sFACES</v>
       </c>
       <c r="F66" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1u5hgykavd7g5nlzgfqhyrt38a74z7t2wufymy4z20fsjjacp6v3s33kqz4</v>
+        <v>https://app.stargaze.zone/launchpad/stars1y7ev7hlvtt6jyhrz3c9zgn760yxhm2hhfnvwl52c85h2e39dn25qr2p5fm</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>stars1kccw8qqpzkj5jcfyh72pycxs2xjfn3r2aa66xg</v>
+        <v>stars1ayw4tr9hcvzvmxucvlay4ewd9qmer9lpecpucy</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>143.00195</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67" t="str">
-        <v>stars1y7ev7hlvtt6jyhrz3c9zgn760yxhm2hhfnvwl52c85h2e39dn25qr2p5fm</v>
+        <v>stars1pny30vz4qe2xmdplk03h7gnrp2q2gqzy8klupk3yjfepe2d8qezqtcl5em</v>
       </c>
       <c r="E67" t="str">
-        <v>sFACES</v>
+        <v>Los Pollos Primos</v>
       </c>
       <c r="F67" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1y7ev7hlvtt6jyhrz3c9zgn760yxhm2hhfnvwl52c85h2e39dn25qr2p5fm</v>
+        <v>https://app.stargaze.zone/launchpad/stars1pny30vz4qe2xmdplk03h7gnrp2q2gqzy8klupk3yjfepe2d8qezqtcl5em</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>stars1ayw4tr9hcvzvmxucvlay4ewd9qmer9lpecpucy</v>
+        <v>stars1ga8afjc392mp88q5aspv9zj2ahgaqh49k6knpu</v>
       </c>
       <c r="B68">
-        <v>139.70195</v>
+        <v>44.999814</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68" t="str">
-        <v>stars1pny30vz4qe2xmdplk03h7gnrp2q2gqzy8klupk3yjfepe2d8qezqtcl5em</v>
+        <v>stars1a5e4tm9rfe8w68w0pdhhcx6rqk9p25qef2qj0xn0sw4tja8vkzrs4zp8qe</v>
       </c>
       <c r="E68" t="str">
-        <v>Los Pollos Primos</v>
+        <v>Stargaze Burgers</v>
       </c>
       <c r="F68" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1pny30vz4qe2xmdplk03h7gnrp2q2gqzy8klupk3yjfepe2d8qezqtcl5em</v>
+        <v>https://app.stargaze.zone/launchpad/stars1a5e4tm9rfe8w68w0pdhhcx6rqk9p25qef2qj0xn0sw4tja8vkzrs4zp8qe</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>stars1ga8afjc392mp88q5aspv9zj2ahgaqh49k6knpu</v>
+        <v>stars1ghlszu0t5xzcrsesa6gkzzv80q5rgcq585hlpm</v>
       </c>
       <c r="B69">
-        <v>44.999814</v>
+        <v>23.699542</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69" t="str">
-        <v>stars1a5e4tm9rfe8w68w0pdhhcx6rqk9p25qef2qj0xn0sw4tja8vkzrs4zp8qe</v>
+        <v>stars1lkrunks3n8adsymusxy453q2u0ctpkeqmurn55ny6hnenl4px09qd7jl6g</v>
       </c>
       <c r="E69" t="str">
-        <v>Stargaze Burgers</v>
+        <v>ohhNFT.com Presents: The Watchers, Protectors of the Interchain</v>
       </c>
       <c r="F69" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1a5e4tm9rfe8w68w0pdhhcx6rqk9p25qef2qj0xn0sw4tja8vkzrs4zp8qe</v>
+        <v>https://app.stargaze.zone/launchpad/stars1lkrunks3n8adsymusxy453q2u0ctpkeqmurn55ny6hnenl4px09qd7jl6g</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>stars1ghlszu0t5xzcrsesa6gkzzv80q5rgcq585hlpm</v>
+        <v>stars1rrcfdc353hafn39a0vpt9ahey0zq4x3vvkzv2s</v>
       </c>
       <c r="B70">
-        <v>371.148249</v>
+        <v>177.363454</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70" t="str">
-        <v>stars1lkrunks3n8adsymusxy453q2u0ctpkeqmurn55ny6hnenl4px09qd7jl6g</v>
+        <v>stars1caghyr0tknmvjfg7py9pspl7dquy3x2s0gzml3227jlzl9n98zeqxglnvg</v>
       </c>
       <c r="E70" t="str">
-        <v>ohhNFT.com Presents: The Watchers, Protectors of the Interchain</v>
+        <v>Banana Kingdom</v>
       </c>
       <c r="F70" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1lkrunks3n8adsymusxy453q2u0ctpkeqmurn55ny6hnenl4px09qd7jl6g</v>
+        <v>https://app.stargaze.zone/launchpad/stars1caghyr0tknmvjfg7py9pspl7dquy3x2s0gzml3227jlzl9n98zeqxglnvg</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>stars1rrcfdc353hafn39a0vpt9ahey0zq4x3vvkzv2s</v>
+        <v>stars1vkfv5l0y53aetu4ftg6mmwus7740zyzt7j8uq8</v>
       </c>
       <c r="B71">
-        <v>177.363454</v>
+        <v>297.751432</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71" t="str">
-        <v>stars1caghyr0tknmvjfg7py9pspl7dquy3x2s0gzml3227jlzl9n98zeqxglnvg</v>
+        <v>stars1mc8wgr90x2usm3t2fgwvz36tjs38tl6c0ddqqkx4jc5tqcayrshs3m25ts</v>
       </c>
       <c r="E71" t="str">
-        <v>Banana Kingdom</v>
+        <v>Cousins</v>
       </c>
       <c r="F71" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1caghyr0tknmvjfg7py9pspl7dquy3x2s0gzml3227jlzl9n98zeqxglnvg</v>
+        <v>https://app.stargaze.zone/launchpad/stars1mc8wgr90x2usm3t2fgwvz36tjs38tl6c0ddqqkx4jc5tqcayrshs3m25ts</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>stars1vkfv5l0y53aetu4ftg6mmwus7740zyzt7j8uq8</v>
+        <v>stars1ceum85c0qz8vgyyczphw57jcsu69msyvlf5ec2</v>
       </c>
       <c r="B72">
-        <v>297.751432</v>
+        <v>499.50195</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72" t="str">
-        <v>stars1mc8wgr90x2usm3t2fgwvz36tjs38tl6c0ddqqkx4jc5tqcayrshs3m25ts</v>
+        <v>stars1zduxpquusenq3ly2fw2h4wxx62ntsuuperjm5yztu9lqc600zrmq40m982</v>
       </c>
       <c r="E72" t="str">
-        <v>Cousins</v>
+        <v>Cosmic Eggs (Common)</v>
       </c>
       <c r="F72" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1mc8wgr90x2usm3t2fgwvz36tjs38tl6c0ddqqkx4jc5tqcayrshs3m25ts</v>
+        <v>https://app.stargaze.zone/launchpad/stars1zduxpquusenq3ly2fw2h4wxx62ntsuuperjm5yztu9lqc600zrmq40m982</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>stars1ceum85c0qz8vgyyczphw57jcsu69msyvlf5ec2</v>
+        <v>stars1l73gt3lg4uu6qfnhsrxsmqry3xdcmzd6hjzu5x</v>
       </c>
       <c r="B73">
-        <v>499.50195</v>
+        <v>89.316611</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73" t="str">
-        <v>stars1zduxpquusenq3ly2fw2h4wxx62ntsuuperjm5yztu9lqc600zrmq40m982</v>
+        <v>stars1zenms99e9f4rq9wjyms69s7gg0k3th7rdnlu26x3aatac3cqxc0sp6tqf6</v>
       </c>
       <c r="E73" t="str">
-        <v>Cosmic Eggs (Common)</v>
+        <v>Genesis Bears</v>
       </c>
       <c r="F73" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1zduxpquusenq3ly2fw2h4wxx62ntsuuperjm5yztu9lqc600zrmq40m982</v>
+        <v>https://app.stargaze.zone/launchpad/stars1zenms99e9f4rq9wjyms69s7gg0k3th7rdnlu26x3aatac3cqxc0sp6tqf6</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>stars1l73gt3lg4uu6qfnhsrxsmqry3xdcmzd6hjzu5x</v>
+        <v>stars1r54k9k2zmdpxc35g96hsfr5qrdr7jprf4ympym</v>
       </c>
       <c r="B74">
-        <v>89.316611</v>
+        <v>111.68195</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74" t="str">
-        <v>stars1zenms99e9f4rq9wjyms69s7gg0k3th7rdnlu26x3aatac3cqxc0sp6tqf6</v>
+        <v>stars1e2yngndz7ddd6hw2eyvh20t6sk6auw03w998m5f9nt7f5qc0megs6q4kr0</v>
       </c>
       <c r="E74" t="str">
-        <v>Genesis Bears</v>
+        <v>Coffee Drop</v>
       </c>
       <c r="F74" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1zenms99e9f4rq9wjyms69s7gg0k3th7rdnlu26x3aatac3cqxc0sp6tqf6</v>
+        <v>https://app.stargaze.zone/launchpad/stars1e2yngndz7ddd6hw2eyvh20t6sk6auw03w998m5f9nt7f5qc0megs6q4kr0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>stars1r54k9k2zmdpxc35g96hsfr5qrdr7jprf4ympym</v>
+        <v>stars12jat9fhaa40gzhkjeay408sl83a8psurslvrne</v>
       </c>
       <c r="B75">
-        <v>111.68195</v>
+        <v>27.247177</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75" t="str">
-        <v>stars1e2yngndz7ddd6hw2eyvh20t6sk6auw03w998m5f9nt7f5qc0megs6q4kr0</v>
+        <v>stars152un9pe9zsut3cqxj3cfgzn5vf69x6tt8lzch7fxg9au66zsyjeqxuwswu</v>
       </c>
       <c r="E75" t="str">
-        <v>Coffee Drop</v>
+        <v>Cinemaddiction</v>
       </c>
       <c r="F75" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1e2yngndz7ddd6hw2eyvh20t6sk6auw03w998m5f9nt7f5qc0megs6q4kr0</v>
+        <v>https://app.stargaze.zone/launchpad/stars152un9pe9zsut3cqxj3cfgzn5vf69x6tt8lzch7fxg9au66zsyjeqxuwswu</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>stars12jat9fhaa40gzhkjeay408sl83a8psurslvrne</v>
+        <v>stars1p34eqrfqvj6624uj5jw0ewg5s2cs06f59cys35</v>
       </c>
       <c r="B76">
-        <v>17.347177</v>
+        <v>1.2</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76" t="str">
-        <v>stars152un9pe9zsut3cqxj3cfgzn5vf69x6tt8lzch7fxg9au66zsyjeqxuwswu</v>
+        <v>stars1qmn72dmr0fspenqut4acdmze9y0jd8j2gm6tufxdg60az3zf3nzsx2xqx0</v>
       </c>
       <c r="E76" t="str">
-        <v>Cinemaddiction</v>
+        <v>Mutant Punks</v>
       </c>
       <c r="F76" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars152un9pe9zsut3cqxj3cfgzn5vf69x6tt8lzch7fxg9au66zsyjeqxuwswu</v>
+        <v>https://app.stargaze.zone/launchpad/stars1qmn72dmr0fspenqut4acdmze9y0jd8j2gm6tufxdg60az3zf3nzsx2xqx0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>stars1p34eqrfqvj6624uj5jw0ewg5s2cs06f59cys35</v>
+        <v>stars1xgjqst7xvakq3rut8syac96tax79np85zvg83w</v>
       </c>
       <c r="B77">
-        <v>4.75</v>
+        <v>499.743731</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77" t="str">
-        <v>stars1qmn72dmr0fspenqut4acdmze9y0jd8j2gm6tufxdg60az3zf3nzsx2xqx0</v>
+        <v>stars16ges8uxkq87zc75fxxq0adv0cl7cp3lqre5fr2xllwysfdegxm7s3rvu4r</v>
       </c>
       <c r="E77" t="str">
-        <v>Mutant Punks</v>
+        <v>Nazar NFT</v>
       </c>
       <c r="F77" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1qmn72dmr0fspenqut4acdmze9y0jd8j2gm6tufxdg60az3zf3nzsx2xqx0</v>
+        <v>https://app.stargaze.zone/launchpad/stars16ges8uxkq87zc75fxxq0adv0cl7cp3lqre5fr2xllwysfdegxm7s3rvu4r</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>stars1xgjqst7xvakq3rut8syac96tax79np85zvg83w</v>
+        <v>stars17vjctfdcyndec6xrdf3l8s8ghfckgked0lamuk</v>
       </c>
       <c r="B78">
-        <v>499.743731</v>
+        <v>445.99913</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78" t="str">
-        <v>stars16ges8uxkq87zc75fxxq0adv0cl7cp3lqre5fr2xllwysfdegxm7s3rvu4r</v>
+        <v>stars1puhek9hsvj9nnk6hxg7mjchh0pxxsuyjxjv5cy8qyjlj4tz7we7s6mclum</v>
       </c>
       <c r="E78" t="str">
-        <v>Nazar NFT</v>
+        <v>888 Voyager Cats</v>
       </c>
       <c r="F78" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars16ges8uxkq87zc75fxxq0adv0cl7cp3lqre5fr2xllwysfdegxm7s3rvu4r</v>
+        <v>https://app.stargaze.zone/launchpad/stars1puhek9hsvj9nnk6hxg7mjchh0pxxsuyjxjv5cy8qyjlj4tz7we7s6mclum</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>stars1qnlpsfmeyl5g6gl6wxz5qggkfyyagtye5tf7sg</v>
+        <v>stars1qkkm73p5wlun2fmllf74e36nkl5uxw4t9gnvda</v>
       </c>
       <c r="B79">
-        <v>1759.551666</v>
+        <v>62.048201</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79" t="str">
-        <v>stars1e55du6h5jvhwhr6p0j0zgw3kdw3q0e2x8sz99teql62yg4rzdu0sgx7xpf</v>
+        <v>stars1jyxv2whtpj4yr30lqs38fkuzk62xsjy8tx3ruv6mr7prjcjln05s0502rn</v>
       </c>
       <c r="E79" t="str">
-        <v>Neural Dither</v>
+        <v>Pepe's Painful Trading Team</v>
       </c>
       <c r="F79" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1e55du6h5jvhwhr6p0j0zgw3kdw3q0e2x8sz99teql62yg4rzdu0sgx7xpf</v>
+        <v>https://app.stargaze.zone/launchpad/stars1jyxv2whtpj4yr30lqs38fkuzk62xsjy8tx3ruv6mr7prjcjln05s0502rn</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>stars17vjctfdcyndec6xrdf3l8s8ghfckgked0lamuk</v>
+        <v>stars14dfhpq7ktv6ew6uf85fhy6t7q50wlrmc9k7dwl</v>
       </c>
       <c r="B80">
-        <v>445.99913</v>
+        <v>1357.12195</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="D80" t="str">
-        <v>stars1puhek9hsvj9nnk6hxg7mjchh0pxxsuyjxjv5cy8qyjlj4tz7we7s6mclum</v>
+        <v>stars1hwd0r4k66e65a7lsgngww3kwuq3rwr2uhvm4wcmgkazuek27qrxqt8gmry</v>
       </c>
       <c r="E80" t="str">
-        <v>888 Voyager Cats</v>
+        <v>Goochi Man Quotes</v>
       </c>
       <c r="F80" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1puhek9hsvj9nnk6hxg7mjchh0pxxsuyjxjv5cy8qyjlj4tz7we7s6mclum</v>
+        <v>https://app.stargaze.zone/launchpad/stars1hwd0r4k66e65a7lsgngww3kwuq3rwr2uhvm4wcmgkazuek27qrxqt8gmry</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>stars1qkkm73p5wlun2fmllf74e36nkl5uxw4t9gnvda</v>
+        <v>stars1d9jlnx840qxlgmvr57m95ujynjccat72huee30</v>
       </c>
       <c r="B81">
-        <v>34.248201</v>
+        <v>225.00195</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81" t="str">
-        <v>stars1jyxv2whtpj4yr30lqs38fkuzk62xsjy8tx3ruv6mr7prjcjln05s0502rn</v>
+        <v>stars1qgx9sf80rv50wgjq0tjym9wga2a5creh5hgrwx9djqky0jhezj8sl38k39</v>
       </c>
       <c r="E81" t="str">
-        <v>Pepe's Painful Trading Team</v>
+        <v>Ghost G</v>
       </c>
       <c r="F81" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1jyxv2whtpj4yr30lqs38fkuzk62xsjy8tx3ruv6mr7prjcjln05s0502rn</v>
+        <v>https://app.stargaze.zone/launchpad/stars1qgx9sf80rv50wgjq0tjym9wga2a5creh5hgrwx9djqky0jhezj8sl38k39</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>stars14dfhpq7ktv6ew6uf85fhy6t7q50wlrmc9k7dwl</v>
+        <v>stars1exce33j7xrd6fmkvyzf3u0887gavdxksh2qlat</v>
       </c>
       <c r="B82">
-        <v>34.75921</v>
+        <v>1003</v>
       </c>
       <c r="C82">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="D82" t="str">
-        <v>stars1hwd0r4k66e65a7lsgngww3kwuq3rwr2uhvm4wcmgkazuek27qrxqt8gmry</v>
+        <v>stars19l9lrzu30tkujeqk8xdj2njfv95zzkaexymlc024lu0auk5kn7tqxhvnqd</v>
       </c>
       <c r="E82" t="str">
-        <v>Goochi Man Quotes</v>
+        <v>Stargaze Citizens</v>
       </c>
       <c r="F82" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1hwd0r4k66e65a7lsgngww3kwuq3rwr2uhvm4wcmgkazuek27qrxqt8gmry</v>
+        <v>https://app.stargaze.zone/launchpad/stars19l9lrzu30tkujeqk8xdj2njfv95zzkaexymlc024lu0auk5kn7tqxhvnqd</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>stars1d9jlnx840qxlgmvr57m95ujynjccat72huee30</v>
+        <v>stars1ycy26n75h7mpalc3x2tjn39g2gctyu5x59aw6g</v>
       </c>
       <c r="B83">
-        <v>225.00195</v>
+        <v>5.566629</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83" t="str">
-        <v>stars1qgx9sf80rv50wgjq0tjym9wga2a5creh5hgrwx9djqky0jhezj8sl38k39</v>
+        <v>stars1xny6xj35q0tm7yf7swemkne4jyvxw0gmde0ud2fgtuazkgnngmas0gcaxc</v>
       </c>
       <c r="E83" t="str">
-        <v>Ghost G</v>
+        <v>Stargaze Gangsters</v>
       </c>
       <c r="F83" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1qgx9sf80rv50wgjq0tjym9wga2a5creh5hgrwx9djqky0jhezj8sl38k39</v>
+        <v>https://app.stargaze.zone/launchpad/stars1xny6xj35q0tm7yf7swemkne4jyvxw0gmde0ud2fgtuazkgnngmas0gcaxc</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>stars1exce33j7xrd6fmkvyzf3u0887gavdxksh2qlat</v>
+        <v>stars1tff5zpw5nnswjstemvr52krcmryvdhc04z3szc</v>
       </c>
       <c r="B84">
-        <v>579.35</v>
+        <v>622.395253</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>1449.049198</v>
       </c>
       <c r="D84" t="str">
-        <v>stars19l9lrzu30tkujeqk8xdj2njfv95zzkaexymlc024lu0auk5kn7tqxhvnqd</v>
+        <v>stars1n2c00l5q03vj3yrh4ndjp5g0tnl9f4fjqqjzawdgxfgv6ejekrxs8r5yjd</v>
       </c>
       <c r="E84" t="str">
-        <v>Stargaze Citizens</v>
+        <v>Moon Plebs</v>
       </c>
       <c r="F84" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars19l9lrzu30tkujeqk8xdj2njfv95zzkaexymlc024lu0auk5kn7tqxhvnqd</v>
+        <v>https://app.stargaze.zone/launchpad/stars1n2c00l5q03vj3yrh4ndjp5g0tnl9f4fjqqjzawdgxfgv6ejekrxs8r5yjd</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>stars1ycy26n75h7mpalc3x2tjn39g2gctyu5x59aw6g</v>
+        <v>stars1g7sueysyd5jv2p73r5tptrsv60haw5fg5am567</v>
       </c>
       <c r="B85">
-        <v>5.566629</v>
+        <v>4.70195</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85" t="str">
-        <v>stars1xny6xj35q0tm7yf7swemkne4jyvxw0gmde0ud2fgtuazkgnngmas0gcaxc</v>
+        <v>stars1xjscx7sg50mr5v96897eashhm8u0ulr9zpkz5h5h97vf0szvw58sftxekf</v>
       </c>
       <c r="E85" t="str">
-        <v>Stargaze Gangsters</v>
+        <v>Cosmo Girls</v>
       </c>
       <c r="F85" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1xny6xj35q0tm7yf7swemkne4jyvxw0gmde0ud2fgtuazkgnngmas0gcaxc</v>
+        <v>https://app.stargaze.zone/launchpad/stars1xjscx7sg50mr5v96897eashhm8u0ulr9zpkz5h5h97vf0szvw58sftxekf</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>stars1tff5zpw5nnswjstemvr52krcmryvdhc04z3szc</v>
+        <v>stars1lzda4yzahhdptpg3cntgwyvxjarufgg2hxzfcq</v>
       </c>
       <c r="B86">
-        <v>608.395253</v>
+        <v>1190.56</v>
       </c>
       <c r="C86">
-        <v>1449.049198</v>
+        <v>0</v>
       </c>
       <c r="D86" t="str">
-        <v>stars1n2c00l5q03vj3yrh4ndjp5g0tnl9f4fjqqjzawdgxfgv6ejekrxs8r5yjd</v>
+        <v>stars16ka9galtk63sza2nhm8ap73vedu4ev090w66kvcrs54r9e4da6uq393c39</v>
       </c>
       <c r="E86" t="str">
-        <v>Moon Plebs</v>
+        <v>Zen Kitties</v>
       </c>
       <c r="F86" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1n2c00l5q03vj3yrh4ndjp5g0tnl9f4fjqqjzawdgxfgv6ejekrxs8r5yjd</v>
+        <v>https://app.stargaze.zone/launchpad/stars16ka9galtk63sza2nhm8ap73vedu4ev090w66kvcrs54r9e4da6uq393c39</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>stars1g7sueysyd5jv2p73r5tptrsv60haw5fg5am567</v>
+        <v>stars1mml7p3qa00mz2ftwyuahun0xhe65nm54sk887j</v>
       </c>
       <c r="B87">
-        <v>4.70195</v>
+        <v>30.156123</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87" t="str">
-        <v>stars1xjscx7sg50mr5v96897eashhm8u0ulr9zpkz5h5h97vf0szvw58sftxekf</v>
+        <v>stars14mp96pt0hg0wyz6k8nmgka060w6eqqenq2g2nuwsm3yq5nzmvk4shnz0my</v>
       </c>
       <c r="E87" t="str">
-        <v>Cosmo Girls</v>
+        <v>Cosmogun</v>
       </c>
       <c r="F87" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1xjscx7sg50mr5v96897eashhm8u0ulr9zpkz5h5h97vf0szvw58sftxekf</v>
+        <v>https://app.stargaze.zone/launchpad/stars14mp96pt0hg0wyz6k8nmgka060w6eqqenq2g2nuwsm3yq5nzmvk4shnz0my</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>stars1lzda4yzahhdptpg3cntgwyvxjarufgg2hxzfcq</v>
+        <v>stars10sxf3mrxlrrerym398sc7e9ps4a0678jskqrkh</v>
       </c>
       <c r="B88">
-        <v>1190.56</v>
+        <v>6.4</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="D88" t="str">
-        <v>stars16ka9galtk63sza2nhm8ap73vedu4ev090w66kvcrs54r9e4da6uq393c39</v>
+        <v>stars1fx9lh2udnzm6nll3kate2pt36z8fppsk0vnq4j6egjysalw4jykqud7w4u</v>
       </c>
       <c r="E88" t="str">
-        <v>Zen Kitties</v>
+        <v>$PACE_MonkeEz</v>
       </c>
       <c r="F88" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars16ka9galtk63sza2nhm8ap73vedu4ev090w66kvcrs54r9e4da6uq393c39</v>
+        <v>https://app.stargaze.zone/launchpad/stars1fx9lh2udnzm6nll3kate2pt36z8fppsk0vnq4j6egjysalw4jykqud7w4u</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>stars1mml7p3qa00mz2ftwyuahun0xhe65nm54sk887j</v>
+        <v>stars1mks5vfqd3lz9zumgdlpwd8zzk0m3kq3h0stk4a</v>
       </c>
       <c r="B89">
-        <v>30.156123</v>
+        <v>35.979624</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>908.962008</v>
       </c>
       <c r="D89" t="str">
-        <v>stars14mp96pt0hg0wyz6k8nmgka060w6eqqenq2g2nuwsm3yq5nzmvk4shnz0my</v>
+        <v>stars1z4v0vnx6sarqx52wrr4v8m3wdqxqm3kgt9v8vc8wxr2juygpxyfq7cayfy</v>
       </c>
       <c r="E89" t="str">
-        <v>Cosmogun</v>
+        <v>Billy Onaires</v>
       </c>
       <c r="F89" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars14mp96pt0hg0wyz6k8nmgka060w6eqqenq2g2nuwsm3yq5nzmvk4shnz0my</v>
+        <v>https://app.stargaze.zone/launchpad/stars1z4v0vnx6sarqx52wrr4v8m3wdqxqm3kgt9v8vc8wxr2juygpxyfq7cayfy</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>stars10sxf3mrxlrrerym398sc7e9ps4a0678jskqrkh</v>
+        <v>stars1vak9fvmyg8txreeezk9p8j94p2yqyafs28hfl9</v>
       </c>
       <c r="B90">
-        <v>6.4</v>
+        <v>1.34675</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90" t="str">
-        <v>stars1fx9lh2udnzm6nll3kate2pt36z8fppsk0vnq4j6egjysalw4jykqud7w4u</v>
+        <v>stars1v9kjyd9exdl9n5t05neg4lqa8a3rwl5rza93msdtnvg77qcmhszskh7z3u</v>
       </c>
       <c r="E90" t="str">
-        <v>$PACE_MonkeEz</v>
+        <v>FORTunate Cookies</v>
       </c>
       <c r="F90" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1fx9lh2udnzm6nll3kate2pt36z8fppsk0vnq4j6egjysalw4jykqud7w4u</v>
+        <v>https://app.stargaze.zone/launchpad/stars1v9kjyd9exdl9n5t05neg4lqa8a3rwl5rza93msdtnvg77qcmhszskh7z3u</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>stars1mks5vfqd3lz9zumgdlpwd8zzk0m3kq3h0stk4a</v>
+        <v>stars158nkavz73whdystnsjl8avufwldt2khufml2ke</v>
       </c>
       <c r="B91">
-        <v>21.719858</v>
+        <v>56.804443</v>
       </c>
       <c r="C91">
-        <v>908.962008</v>
+        <v>11</v>
       </c>
       <c r="D91" t="str">
-        <v>stars1z4v0vnx6sarqx52wrr4v8m3wdqxqm3kgt9v8vc8wxr2juygpxyfq7cayfy</v>
+        <v>stars12vdwd2yzl3hk4l3tsk650w4vdns29n3kl0v5gqgxnapepq9czcmswqq9s9</v>
       </c>
       <c r="E91" t="str">
-        <v>Billy Onaires</v>
+        <v>N/A</v>
       </c>
       <c r="F91" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1z4v0vnx6sarqx52wrr4v8m3wdqxqm3kgt9v8vc8wxr2juygpxyfq7cayfy</v>
+        <v>N/A</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>stars1vak9fvmyg8txreeezk9p8j94p2yqyafs28hfl9</v>
+        <v>stars1r5ecq7zn6hwh5e68e79ume8rp9ht7kjz352drk</v>
       </c>
       <c r="B92">
-        <v>1.34675</v>
+        <v>2645.624528</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92" t="str">
-        <v>stars1v9kjyd9exdl9n5t05neg4lqa8a3rwl5rza93msdtnvg77qcmhszskh7z3u</v>
+        <v>stars1cduudfszcm9slm8qxlaqvnpzg2u0hkus94fe3pwt9x446dtw6eeqrz6q48</v>
       </c>
       <c r="E92" t="str">
-        <v>FORTunate Cookies</v>
+        <v>N/A</v>
       </c>
       <c r="F92" t="str">
-        <v>https://app.stargaze.zone/launchpad/stars1v9kjyd9exdl9n5t05neg4lqa8a3rwl5rza93msdtnvg77qcmhszskh7z3u</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="str">
-        <v>stars158nkavz73whdystnsjl8avufwldt2khufml2ke</v>
-      </c>
-      <c r="B93">
-        <v>56.804443</v>
-      </c>
-      <c r="C93">
-        <v>11</v>
-      </c>
-      <c r="D93" t="str">
-        <v>stars12vdwd2yzl3hk4l3tsk650w4vdns29n3kl0v5gqgxnapepq9czcmswqq9s9</v>
-      </c>
-      <c r="E93" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="F93" t="str">
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="str">
-        <v>stars1r5ecq7zn6hwh5e68e79ume8rp9ht7kjz352drk</v>
-      </c>
-      <c r="B94">
-        <v>3645.626702</v>
-      </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-      <c r="D94" t="str">
-        <v>stars1cduudfszcm9slm8qxlaqvnpzg2u0hkus94fe3pwt9x446dtw6eeqrz6q48</v>
-      </c>
-      <c r="E94" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="F94" t="str">
         <v>N/A</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F94"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F92"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>